<commit_message>
Changed naming deliminator to keep bird ids from entering other columns if names consisted of multiple words
</commit_message>
<xml_diff>
--- a/Outside_small.xlsx
+++ b/Outside_small.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\batra\Documents\Emily Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15700CB8-BCEC-4A00-8EFE-862CDA221FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F43AF6D-3E76-4BB4-B8F3-D1AA9F6BA8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,9 +94,6 @@
     <t>Standard deviation</t>
   </si>
   <si>
-    <t>cactus_wren_ventral_4_2024-01-16_10-37-45</t>
-  </si>
-  <si>
     <t>belly_dark</t>
   </si>
   <si>
@@ -136,13 +133,7 @@
     <t>back_full</t>
   </si>
   <si>
-    <t>palm_tanager_ventral_7_2024-01-16_10-40-53</t>
-  </si>
-  <si>
     <t>breast</t>
-  </si>
-  <si>
-    <t>ramphocelus_n_ventral_8_2024-01-16_10-42-04</t>
   </si>
   <si>
     <t>throat</t>
@@ -157,25 +148,13 @@
     <t>breast2</t>
   </si>
   <si>
-    <t>ramphocelus_n_dorsal_9_2024-01-16_10-42-52</t>
-  </si>
-  <si>
     <t>nape1</t>
   </si>
   <si>
     <t>nape2</t>
   </si>
   <si>
-    <t>ramphocelus_c_ventral_10_2024-01-16_10-43-33</t>
-  </si>
-  <si>
     <t>belly</t>
-  </si>
-  <si>
-    <t>Darwin's_finch_ventral_11_2024-01-16_10-44-43</t>
-  </si>
-  <si>
-    <t>House_finch_ventral_12_2024-01-16_10-46-22</t>
   </si>
   <si>
     <t>munia_ventral_14_2024-01-16_10-48-04</t>
@@ -190,28 +169,49 @@
     <t>flank_full</t>
   </si>
   <si>
-    <t>alan's_hummingbird_ventral_15_2024-01-16_10-49-09</t>
-  </si>
-  <si>
-    <t>alan's_hummingbird_dorsal_16_2024-01-16_10-49-46</t>
-  </si>
-  <si>
     <t>back</t>
-  </si>
-  <si>
-    <t>alan's_hummingbird_dorsal_2_17_2024-01-16_10-50-50</t>
   </si>
   <si>
     <t>back2</t>
   </si>
   <si>
-    <t>fiery_throated_hummingbird_ventral_18_2024-01-16_10-51-46</t>
-  </si>
-  <si>
     <t>belly_to_throat</t>
   </si>
   <si>
-    <t>tanager_ventral_2_3_2024-01-16_10-36-53</t>
+    <t>cactus.wren_ventral_4_2024-01-16_10-37-45</t>
+  </si>
+  <si>
+    <t>palm.tanager_ventral_7_2024-01-16_10-40-53</t>
+  </si>
+  <si>
+    <t>ramphocelus.n_ventral_8_2024-01-16_10-42-04</t>
+  </si>
+  <si>
+    <t>ramphocelus.n_dorsal_9_2024-01-16_10-42-52</t>
+  </si>
+  <si>
+    <t>ramphocelus.c_ventral_10_2024-01-16_10-43-33</t>
+  </si>
+  <si>
+    <t>Darwin's.finch_ventral_11_2024-01-16_10-44-43</t>
+  </si>
+  <si>
+    <t>House.finch_ventral_12_2024-01-16_10-46-22</t>
+  </si>
+  <si>
+    <t>alan's.hummingbird_ventral_15_2024-01-16_10-49-09</t>
+  </si>
+  <si>
+    <t>alan's.hummingbird_dorsal_16_2024-01-16_10-49-46</t>
+  </si>
+  <si>
+    <t>alan's.hummingbird_dorsal_2_17_2024-01-16_10-50-50</t>
+  </si>
+  <si>
+    <t>fiery.throated.hummingbird_ventral_18_2024-01-16_10-51-46</t>
+  </si>
+  <si>
+    <t>summer.tanager_ventral_2_3_2024-01-16_10-36-53</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:MB38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2651,10 +2653,10 @@
     </row>
     <row r="7" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
       </c>
       <c r="C7">
         <v>292</v>
@@ -2669,7 +2671,7 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -3664,10 +3666,10 @@
     </row>
     <row r="8" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>252</v>
@@ -3682,7 +3684,7 @@
         <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -4677,10 +4679,10 @@
     </row>
     <row r="9" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>238</v>
@@ -4695,7 +4697,7 @@
         <v>112</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -5690,10 +5692,10 @@
     </row>
     <row r="10" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
       </c>
       <c r="C10">
         <v>282</v>
@@ -5708,7 +5710,7 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -6703,10 +6705,10 @@
     </row>
     <row r="11" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>265</v>
@@ -6721,7 +6723,7 @@
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -7716,10 +7718,10 @@
     </row>
     <row r="12" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
       </c>
       <c r="C12">
         <v>250</v>
@@ -7734,7 +7736,7 @@
         <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -8729,10 +8731,10 @@
     </row>
     <row r="13" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <v>264</v>
@@ -8747,7 +8749,7 @@
         <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -9742,10 +9744,10 @@
     </row>
     <row r="14" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14">
         <v>267</v>
@@ -9760,7 +9762,7 @@
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -10755,10 +10757,10 @@
     </row>
     <row r="15" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <v>222</v>
@@ -10773,7 +10775,7 @@
         <v>142</v>
       </c>
       <c r="G15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -11768,10 +11770,10 @@
     </row>
     <row r="16" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>229</v>
@@ -11786,7 +11788,7 @@
         <v>51</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -12781,10 +12783,10 @@
     </row>
     <row r="17" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17">
         <v>254</v>
@@ -12799,7 +12801,7 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
@@ -13794,10 +13796,10 @@
     </row>
     <row r="18" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C18">
         <v>247</v>
@@ -13812,7 +13814,7 @@
         <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -14807,10 +14809,10 @@
     </row>
     <row r="19" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
         <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
       </c>
       <c r="C19">
         <v>230</v>
@@ -14825,7 +14827,7 @@
         <v>35</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -15820,10 +15822,10 @@
     </row>
     <row r="20" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C20">
         <v>333</v>
@@ -15838,7 +15840,7 @@
         <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -16833,10 +16835,10 @@
     </row>
     <row r="21" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C21">
         <v>220</v>
@@ -16851,7 +16853,7 @@
         <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
@@ -17846,10 +17848,10 @@
     </row>
     <row r="22" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <v>246</v>
@@ -17864,7 +17866,7 @@
         <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -18859,10 +18861,10 @@
     </row>
     <row r="23" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C23">
         <v>273</v>
@@ -18877,7 +18879,7 @@
         <v>55</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
@@ -19872,10 +19874,10 @@
     </row>
     <row r="24" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C24">
         <v>247</v>
@@ -19890,7 +19892,7 @@
         <v>92</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
@@ -20885,10 +20887,10 @@
     </row>
     <row r="25" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25">
         <v>243</v>
@@ -20903,7 +20905,7 @@
         <v>42</v>
       </c>
       <c r="G25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -21898,10 +21900,10 @@
     </row>
     <row r="26" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C26">
         <v>294</v>
@@ -21916,7 +21918,7 @@
         <v>21</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -22911,10 +22913,10 @@
     </row>
     <row r="27" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C27">
         <v>294</v>
@@ -22929,7 +22931,7 @@
         <v>18</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -23924,10 +23926,10 @@
     </row>
     <row r="28" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C28">
         <v>346</v>
@@ -23942,7 +23944,7 @@
         <v>4</v>
       </c>
       <c r="G28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -24937,10 +24939,10 @@
     </row>
     <row r="29" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C29">
         <v>354</v>
@@ -24955,7 +24957,7 @@
         <v>9</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -25950,10 +25952,10 @@
     </row>
     <row r="30" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C30">
         <v>314</v>
@@ -25968,7 +25970,7 @@
         <v>62</v>
       </c>
       <c r="G30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
@@ -26963,10 +26965,10 @@
     </row>
     <row r="31" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C31">
         <v>283</v>
@@ -26981,7 +26983,7 @@
         <v>31</v>
       </c>
       <c r="G31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -27976,10 +27978,10 @@
     </row>
     <row r="32" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C32">
         <v>261</v>
@@ -27994,7 +27996,7 @@
         <v>76</v>
       </c>
       <c r="G32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
@@ -28989,10 +28991,10 @@
     </row>
     <row r="33" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C33">
         <v>281</v>
@@ -29007,7 +29009,7 @@
         <v>97</v>
       </c>
       <c r="G33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
@@ -30002,10 +30004,10 @@
     </row>
     <row r="34" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C34">
         <v>306</v>
@@ -30020,7 +30022,7 @@
         <v>30</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I34" t="b">
         <v>1</v>
@@ -31015,10 +31017,10 @@
     </row>
     <row r="35" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C35">
         <v>286</v>
@@ -31033,7 +31035,7 @@
         <v>57</v>
       </c>
       <c r="G35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I35" t="b">
         <v>1</v>
@@ -32028,10 +32030,10 @@
     </row>
     <row r="36" spans="1:340" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C36">
         <v>297</v>
@@ -32046,7 +32048,7 @@
         <v>136</v>
       </c>
       <c r="G36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -33044,7 +33046,7 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C37">
         <v>219</v>
@@ -33059,7 +33061,7 @@
         <v>44</v>
       </c>
       <c r="G37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I37" t="b">
         <v>1</v>
@@ -34057,7 +34059,7 @@
         <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C38">
         <v>252</v>
@@ -34072,7 +34074,7 @@
         <v>76</v>
       </c>
       <c r="G38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>

</xml_diff>